<commit_message>
Images are extracted and thermal calculations are updated.
</commit_message>
<xml_diff>
--- a/Thermal Calculation.xlsx
+++ b/Thermal Calculation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\EE463\METU-EEE-463-Term-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{020EE09A-A5CE-4B84-8A7E-D550CDD8FD69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59A98CB-3F9B-428D-8B49-F9AC9A0A0CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{EA438769-6E61-4BE8-9A6F-BFF01EB0C246}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EA438769-6E61-4BE8-9A6F-BFF01EB0C246}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
   <si>
     <t>PSW (W)</t>
   </si>
@@ -130,6 +130,15 @@
   </si>
   <si>
     <t>T ambient new (C)</t>
+  </si>
+  <si>
+    <t>Heatsink Thermal with fan</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>Currents (A)</t>
   </si>
 </sst>
 </file>
@@ -139,7 +148,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,8 +174,15 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +198,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -288,16 +310,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -307,16 +340,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -326,13 +349,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,6 +373,1174 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="tr-TR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="tr-TR"/>
+              <a:t>Estimated</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="tr-TR" baseline="0"/>
+              <a:t> Junction Temperature</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="tr-TR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sayfa1!$P$6:$P$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sayfa1!$U$6:$U$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>25.183149999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.609299999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.035449999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35.461599999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38.887749999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42.313899999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45.740049999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>49.166199999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>52.592349999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>56.018499999999989</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>59.444649999999989</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>62.870799999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>66.296949999999981</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>69.723099999999988</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>73.149249999999995</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>76.575400000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80.00154999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>83.427699999999987</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>86.85384999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>90.279999999999987</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>93.70614999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>97.132299999999987</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>100.55844999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>103.9846</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>107.41074999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1F4F-4F19-BA27-9AAB4B7AF723}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1298820559"/>
+        <c:axId val="1298816815"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1298820559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="tr-TR"/>
+                  <a:t>Current (A)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="tr-TR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="tr-TR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1298816815"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1298816815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="tr-TR"/>
+                  <a:t>Function Temperature (C)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="tr-TR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="tr-TR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1298820559"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="tr-TR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>198391</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>85453</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>535304</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>165191</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7641F80B-33DD-45E3-8D43-6279B61A4EB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -648,57 +1840,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F0EFF5B-56C1-4C62-9997-8962C5724F41}">
-  <dimension ref="B3:J40"/>
+  <dimension ref="B3:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AE36" sqref="AE36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.7109375" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C3" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="P5" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="G6" s="14" t="s">
+        <v>0.4</v>
+      </c>
+      <c r="G6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="16"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="21"/>
       <c r="J6" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="R6" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S6" s="12">
+        <f>D10*P6*D12</f>
+        <v>1.365</v>
+      </c>
+      <c r="T6" s="12">
+        <f>R6+S6</f>
+        <v>2.0649999999999999</v>
+      </c>
+      <c r="U6" s="24">
+        <f>(D13+D14+D15)*T6+C3</f>
+        <v>25.183149999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="17"/>
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="2">
-        <v>0.63</v>
+        <v>0.3</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>0</v>
@@ -712,95 +1943,297 @@
       <c r="J7" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
+      <c r="P7">
+        <v>2</v>
+      </c>
+      <c r="R7" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S7">
+        <f>D10*P7*D12</f>
+        <v>2.73</v>
+      </c>
+      <c r="T7" s="12">
+        <f t="shared" ref="T7:T30" si="0">R7+S7</f>
+        <v>3.4299999999999997</v>
+      </c>
+      <c r="U7" s="24">
+        <f>(D13+D14+D15)*T7+C3</f>
+        <v>28.609299999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="17"/>
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="3">
-        <v>10000</v>
-      </c>
-      <c r="G8" s="18">
+        <v>1000</v>
+      </c>
+      <c r="G8" s="10">
         <f>(D6+D7)/1000*D8</f>
-        <v>11.299999999999999</v>
-      </c>
-      <c r="H8" s="19">
+        <v>0.7</v>
+      </c>
+      <c r="H8" s="11">
         <f>D10*D11*D12</f>
-        <v>22.814999999999998</v>
-      </c>
-      <c r="I8" s="20">
+        <v>13.649999999999999</v>
+      </c>
+      <c r="I8" s="12">
         <f>G8+H8</f>
-        <v>34.114999999999995</v>
-      </c>
-      <c r="J8" s="23">
+        <v>14.349999999999998</v>
+      </c>
+      <c r="J8" s="15">
         <f>I8*(D13+D14+D15)+C3</f>
-        <v>166.91839999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
+        <v>56.018499999999989</v>
+      </c>
+      <c r="P8">
+        <v>3</v>
+      </c>
+      <c r="R8" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S8">
+        <f>D10*P8*D12</f>
+        <v>4.0949999999999998</v>
+      </c>
+      <c r="T8" s="12">
+        <f t="shared" si="0"/>
+        <v>4.7949999999999999</v>
+      </c>
+      <c r="U8" s="24">
+        <f>(D13+D14+D15)*T8+C3</f>
+        <v>32.035449999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="17"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
+      <c r="P9">
+        <v>4</v>
+      </c>
+      <c r="R9" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S9">
+        <f>D10*P9*D12</f>
+        <v>5.46</v>
+      </c>
+      <c r="T9" s="12">
+        <f t="shared" si="0"/>
+        <v>6.16</v>
+      </c>
+      <c r="U9" s="24">
+        <f>(D13+D14+D15)*T9+C3</f>
+        <v>35.461599999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="17"/>
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="4">
         <v>1.95</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
+      <c r="P10">
+        <v>5</v>
+      </c>
+      <c r="R10" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S10">
+        <f>D10*P10*D12</f>
+        <v>6.8249999999999993</v>
+      </c>
+      <c r="T10" s="12">
+        <f t="shared" si="0"/>
+        <v>7.5249999999999995</v>
+      </c>
+      <c r="U10" s="24">
+        <f>(D13+D14+D15)*T10+C3</f>
+        <v>38.887749999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B11" s="17"/>
       <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
+        <v>10</v>
+      </c>
+      <c r="P11">
+        <v>6</v>
+      </c>
+      <c r="R11" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S11">
+        <f>D10*P11*D12</f>
+        <v>8.19</v>
+      </c>
+      <c r="T11" s="12">
+        <f t="shared" si="0"/>
+        <v>8.8899999999999988</v>
+      </c>
+      <c r="U11" s="24">
+        <f>(D13+D14+D15)*T11+C3</f>
+        <v>42.313899999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="17"/>
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="4">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
+        <v>0.7</v>
+      </c>
+      <c r="P12">
+        <v>7</v>
+      </c>
+      <c r="R12" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S12">
+        <f>D10*P12*D12</f>
+        <v>9.5549999999999997</v>
+      </c>
+      <c r="T12" s="12">
+        <f t="shared" si="0"/>
+        <v>10.254999999999999</v>
+      </c>
+      <c r="U12" s="24">
+        <f>(D13+D14+D15)*T12+C3</f>
+        <v>45.740049999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B13" s="17"/>
       <c r="C13" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="4">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="9"/>
+      <c r="P13">
+        <v>8</v>
+      </c>
+      <c r="R13" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S13">
+        <f>D10*P13*D12</f>
+        <v>10.92</v>
+      </c>
+      <c r="T13" s="12">
+        <f t="shared" si="0"/>
+        <v>11.62</v>
+      </c>
+      <c r="U13" s="24">
+        <f>(D13+D14+D15)*T13+C3</f>
+        <v>49.166199999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14" s="18"/>
       <c r="C14" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="4">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <v>9</v>
+      </c>
+      <c r="R14" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S14">
+        <f>D10*P14*D12</f>
+        <v>12.285</v>
+      </c>
+      <c r="T14" s="12">
+        <f t="shared" si="0"/>
+        <v>12.984999999999999</v>
+      </c>
+      <c r="U14" s="24">
+        <f>(D13+D14+D15)*T14+C3</f>
+        <v>52.592349999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="13">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
+        <v>1.65</v>
+      </c>
+      <c r="P15">
+        <v>10</v>
+      </c>
+      <c r="R15" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S15">
+        <f>D10*P15*D12</f>
+        <v>13.649999999999999</v>
+      </c>
+      <c r="T15" s="12">
+        <f t="shared" si="0"/>
+        <v>14.349999999999998</v>
+      </c>
+      <c r="U15" s="24">
+        <f>(D13+D14+D15)*T15+C3</f>
+        <v>56.018499999999989</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <v>11</v>
+      </c>
+      <c r="R16" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S16">
+        <f>D10*P16*D12</f>
+        <v>15.014999999999999</v>
+      </c>
+      <c r="T16" s="12">
+        <f t="shared" si="0"/>
+        <v>15.714999999999998</v>
+      </c>
+      <c r="U16" s="24">
+        <f>(D13+D14+D15)*T16+C3</f>
+        <v>59.444649999999989</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <v>12</v>
+      </c>
+      <c r="R17" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S17">
+        <f>D10*P17*D12</f>
+        <v>16.38</v>
+      </c>
+      <c r="T17" s="12">
+        <f t="shared" si="0"/>
+        <v>17.079999999999998</v>
+      </c>
+      <c r="U17" s="24">
+        <f>(D13+D14+D15)*T17+C3</f>
+        <v>62.870799999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="23" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -809,27 +2242,45 @@
       <c r="D18" s="4">
         <v>200</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
       <c r="J18" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
+      <c r="P18">
+        <v>13</v>
+      </c>
+      <c r="R18" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S18">
+        <f>D10*P18*D12</f>
+        <v>17.744999999999997</v>
+      </c>
+      <c r="T18" s="12">
+        <f t="shared" si="0"/>
+        <v>18.444999999999997</v>
+      </c>
+      <c r="U18" s="24">
+        <f>(D13+D14+D15)*T18+C3</f>
+        <v>66.296949999999981</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="23"/>
       <c r="C19" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="4">
-        <v>10000</v>
-      </c>
-      <c r="G19" s="17" t="s">
+        <v>1000</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H19" s="9" t="s">
         <v>5</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -838,104 +2289,324 @@
       <c r="J19" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
+      <c r="P19">
+        <v>14</v>
+      </c>
+      <c r="R19" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S19">
+        <f>D10*P19*D12</f>
+        <v>19.11</v>
+      </c>
+      <c r="T19" s="12">
+        <f t="shared" si="0"/>
+        <v>19.809999999999999</v>
+      </c>
+      <c r="U19" s="24">
+        <f>(D13+D14+D15)*T19+C3</f>
+        <v>69.723099999999988</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="23"/>
       <c r="C20" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="4">
         <v>35</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="11">
         <f>D18*D19*D20/1000000000*D21/1000000</f>
-        <v>7.0000000000000007E-6</v>
-      </c>
-      <c r="H20" s="19">
+        <v>7.0000000000000007E-7</v>
+      </c>
+      <c r="H20" s="11">
         <f>D23*D24*D25</f>
-        <v>15.678000000000003</v>
-      </c>
-      <c r="I20" s="19">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="I20" s="11">
         <f>G20+H20</f>
-        <v>15.678007000000003</v>
-      </c>
-      <c r="J20" s="22">
+        <v>4.0200006999999998</v>
+      </c>
+      <c r="J20" s="14">
         <f>I20*(D26+D27+D28)+C3</f>
-        <v>95.551031500000008</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
+        <v>31.457001994999999</v>
+      </c>
+      <c r="P20">
+        <v>15</v>
+      </c>
+      <c r="R20" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S20">
+        <f>D10*P20*D12</f>
+        <v>20.474999999999998</v>
+      </c>
+      <c r="T20" s="12">
+        <f t="shared" si="0"/>
+        <v>21.174999999999997</v>
+      </c>
+      <c r="U20" s="24">
+        <f>(D13+D14+D15)*T20+C3</f>
+        <v>73.149249999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="23"/>
       <c r="C21" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="4">
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="12"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
+      <c r="P21">
+        <v>16</v>
+      </c>
+      <c r="R21" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S21">
+        <f>D10*P21*D12</f>
+        <v>21.84</v>
+      </c>
+      <c r="T21" s="12">
+        <f t="shared" si="0"/>
+        <v>22.54</v>
+      </c>
+      <c r="U21" s="24">
+        <f>(D13+D14+D15)*T21+C3</f>
+        <v>76.575400000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B22" s="23"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="7"/>
+      <c r="P22">
+        <v>17</v>
+      </c>
+      <c r="R22" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S22">
+        <f>D10*P22*D12</f>
+        <v>23.204999999999998</v>
+      </c>
+      <c r="T22" s="12">
+        <f t="shared" si="0"/>
+        <v>23.904999999999998</v>
+      </c>
+      <c r="U22" s="24">
+        <f>(D13+D14+D15)*T22+C3</f>
+        <v>80.00154999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B23" s="23"/>
       <c r="C23" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="4">
         <v>1.34</v>
       </c>
-    </row>
-    <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
+      <c r="P23">
+        <v>18</v>
+      </c>
+      <c r="R23" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S23">
+        <f>D10*P23*D12</f>
+        <v>24.57</v>
+      </c>
+      <c r="T23" s="12">
+        <f t="shared" si="0"/>
+        <v>25.27</v>
+      </c>
+      <c r="U23" s="24">
+        <f>(D13+D14+D15)*T23+C3</f>
+        <v>83.427699999999987</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="23"/>
       <c r="C24" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D24" s="4">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="P24">
+        <v>19</v>
+      </c>
+      <c r="R24" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S24">
+        <f>D10*P24*D12</f>
+        <v>25.934999999999995</v>
+      </c>
+      <c r="T24" s="12">
+        <f t="shared" si="0"/>
+        <v>26.634999999999994</v>
+      </c>
+      <c r="U24" s="24">
+        <f>(D13+D14+D15)*T24+C3</f>
+        <v>86.85384999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B25" s="23"/>
       <c r="C25" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="4">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
+        <v>0.3</v>
+      </c>
+      <c r="P25">
+        <v>20</v>
+      </c>
+      <c r="R25" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S25">
+        <f>D10*P25*D12</f>
+        <v>27.299999999999997</v>
+      </c>
+      <c r="T25" s="12">
+        <f t="shared" si="0"/>
+        <v>27.999999999999996</v>
+      </c>
+      <c r="U25" s="24">
+        <f>(D13+D14+D15)*T25+C3</f>
+        <v>90.279999999999987</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B26" s="23"/>
       <c r="C26" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="4">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
+      <c r="P26">
+        <v>21</v>
+      </c>
+      <c r="R26" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S26">
+        <f>D10*P26*D12</f>
+        <v>28.664999999999996</v>
+      </c>
+      <c r="T26" s="12">
+        <f t="shared" si="0"/>
+        <v>29.364999999999995</v>
+      </c>
+      <c r="U26" s="24">
+        <f>(D13+D14+D15)*T26+C3</f>
+        <v>93.70614999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="23"/>
       <c r="C27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27" s="8">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="P27">
+        <v>22</v>
+      </c>
+      <c r="R27" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S27">
+        <f>D10*P27*D12</f>
+        <v>30.029999999999998</v>
+      </c>
+      <c r="T27" s="12">
+        <f t="shared" si="0"/>
+        <v>30.729999999999997</v>
+      </c>
+      <c r="U27" s="24">
+        <f>(D13+D14+D15)*T27+C3</f>
+        <v>97.132299999999987</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="13">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="6" t="s">
+      <c r="D28" s="8">
+        <v>1.65</v>
+      </c>
+      <c r="P28">
+        <v>23</v>
+      </c>
+      <c r="R28" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S28">
+        <f>D10*P28*D12</f>
+        <v>31.395</v>
+      </c>
+      <c r="T28" s="12">
+        <f t="shared" si="0"/>
+        <v>32.094999999999999</v>
+      </c>
+      <c r="U28" s="24">
+        <f>(D13+D14+D15)*T28+C3</f>
+        <v>100.55844999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="P29">
+        <v>24</v>
+      </c>
+      <c r="R29" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S29">
+        <f>D10*P29*D12</f>
+        <v>32.76</v>
+      </c>
+      <c r="T29" s="12">
+        <f t="shared" si="0"/>
+        <v>33.46</v>
+      </c>
+      <c r="U29" s="24">
+        <f>(D13+D14+D15)*T29+C3</f>
+        <v>103.9846</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="P30">
+        <v>25</v>
+      </c>
+      <c r="R30" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="S30">
+        <f>D10*P30*D12</f>
+        <v>34.125</v>
+      </c>
+      <c r="T30" s="12">
+        <f t="shared" si="0"/>
+        <v>34.825000000000003</v>
+      </c>
+      <c r="U30" s="24">
+        <f>(D13+D14+D15)*T30+C3</f>
+        <v>107.41074999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B31" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C31" s="5" t="s">
@@ -944,17 +2615,17 @@
       <c r="D31" s="4">
         <v>235</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H31" s="15"/>
-      <c r="I31" s="16"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="21"/>
       <c r="J31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="6"/>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B32" s="23"/>
       <c r="C32" s="5" t="s">
         <v>3</v>
       </c>
@@ -975,32 +2646,29 @@
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="6"/>
+      <c r="B33" s="23"/>
       <c r="C33" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D33" s="4">
         <v>50</v>
       </c>
-      <c r="G33" s="19">
-        <f>D31*D32*D33/1000000000*D34/1000000</f>
-        <v>5.8749999999999997E-9</v>
-      </c>
-      <c r="H33" s="19">
-        <f>D37*D36</f>
-        <v>15.6</v>
-      </c>
-      <c r="I33" s="19">
-        <f>G33+H33</f>
-        <v>15.600000005875</v>
-      </c>
-      <c r="J33" s="22">
+      <c r="G33" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I33" s="11">
+        <v>20</v>
+      </c>
+      <c r="J33" s="14">
         <f>I33*(D38+D39+D40)+C3</f>
-        <v>97.696000027377494</v>
+        <v>80.199999999999989</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="6"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="5" t="s">
         <v>20</v>
       </c>
@@ -1009,12 +2677,12 @@
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="6"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="12"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="7"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="6"/>
+      <c r="B36" s="23"/>
       <c r="C36" s="5" t="s">
         <v>21</v>
       </c>
@@ -1023,7 +2691,7 @@
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="6"/>
+      <c r="B37" s="23"/>
       <c r="C37" s="5" t="s">
         <v>22</v>
       </c>
@@ -1032,7 +2700,7 @@
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="6"/>
+      <c r="B38" s="23"/>
       <c r="C38" s="5" t="s">
         <v>24</v>
       </c>
@@ -1041,11 +2709,11 @@
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="6"/>
+      <c r="B39" s="23"/>
       <c r="C39" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="21">
+      <c r="D39" s="13">
         <v>0.2</v>
       </c>
     </row>
@@ -1056,8 +2724,8 @@
       <c r="C40" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="21">
-        <v>3.3</v>
+      <c r="D40" s="13">
+        <v>1.65</v>
       </c>
     </row>
   </sheetData>
@@ -1071,5 +2739,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>